<commit_message>
More fixes and cleaning to data aggregation.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Note_sheet_AM.xlsx
+++ b/raw-data-prep/raw_data/Note_sheet_AM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -278,9 +278,6 @@
     <t>Did not wear headphones for full 15 minutes; No suspicions about study</t>
   </si>
   <si>
-    <t>What is study about?: Effect of distraction on video game playing; Anything suspicious?" "maybe we were writing the essay responses to distract the more"; laughed when gave distraction assignment;  Essay review was too much "A normal person isn't that mean"</t>
-  </si>
-  <si>
     <t>Mallory</t>
   </si>
   <si>
@@ -324,13 +321,16 @@
   </si>
   <si>
     <t>Game 1</t>
+  </si>
+  <si>
+    <t>Study about effect of distraction on video game playing. Anything suspicious: maybe we were writing the essay responses to distract the more. laughed when gave distraction assignment. Said essay review was too much. A normal person isn't that mean.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,6 +526,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -560,6 +561,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -735,21 +737,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="N74" sqref="N74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -769,19 +771,19 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H1" t="s">
         <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J1" t="s">
         <v>13</v>
       </c>
       <c r="K1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L1" t="s">
         <v>14</v>
@@ -790,10 +792,10 @@
         <v>6</v>
       </c>
       <c r="N1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>41550</v>
       </c>
@@ -834,7 +836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickTop="1">
+    <row r="3" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>41547</v>
       </c>
@@ -875,7 +877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>41541</v>
       </c>
@@ -919,7 +921,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>41545</v>
       </c>
@@ -963,7 +965,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>41550</v>
       </c>
@@ -1004,7 +1006,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>41545</v>
       </c>
@@ -1048,7 +1050,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>41541</v>
       </c>
@@ -1089,7 +1091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>41541</v>
       </c>
@@ -1130,7 +1132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>41542</v>
       </c>
@@ -1174,7 +1176,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>41542</v>
       </c>
@@ -1215,7 +1217,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
+    <row r="12" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>41543</v>
       </c>
@@ -1259,7 +1261,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickTop="1">
+    <row r="13" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>41543</v>
       </c>
@@ -1300,7 +1302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>41543</v>
       </c>
@@ -1341,7 +1343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
+    <row r="15" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>41543</v>
       </c>
@@ -1382,7 +1384,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickTop="1">
+    <row r="16" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>41543</v>
       </c>
@@ -1423,7 +1425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>41543</v>
       </c>
@@ -1464,7 +1466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>41544</v>
       </c>
@@ -1508,7 +1510,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>41544</v>
       </c>
@@ -1552,7 +1554,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1596,7 +1598,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>41545</v>
       </c>
@@ -1640,7 +1642,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>41545</v>
       </c>
@@ -1684,7 +1686,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>41546</v>
       </c>
@@ -1728,7 +1730,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>41546</v>
       </c>
@@ -1772,7 +1774,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>41547</v>
       </c>
@@ -1816,7 +1818,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>41548</v>
       </c>
@@ -1857,7 +1859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>41548</v>
       </c>
@@ -1901,7 +1903,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1942,7 +1944,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>41548</v>
       </c>
@@ -1986,7 +1988,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>41549</v>
       </c>
@@ -2027,7 +2029,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>41549</v>
       </c>
@@ -2068,7 +2070,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -2109,7 +2111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>41549</v>
       </c>
@@ -2153,7 +2155,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>41550</v>
       </c>
@@ -2194,7 +2196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
+    <row r="35" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>41550</v>
       </c>
@@ -2235,7 +2237,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickTop="1">
+    <row r="36" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>41550</v>
       </c>
@@ -2276,7 +2278,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>41550</v>
       </c>
@@ -2317,7 +2319,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>41550</v>
       </c>
@@ -2361,7 +2363,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>41551</v>
       </c>
@@ -2402,7 +2404,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" thickBot="1">
+    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>41551</v>
       </c>
@@ -2446,7 +2448,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
+    <row r="41" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>41551</v>
       </c>
@@ -2487,7 +2489,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15.75" thickTop="1">
+    <row r="42" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>41936</v>
       </c>
@@ -2531,7 +2533,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>41936</v>
       </c>
@@ -2575,7 +2577,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>41936</v>
       </c>
@@ -2619,7 +2621,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>41936</v>
       </c>
@@ -2663,7 +2665,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>41936</v>
       </c>
@@ -2707,7 +2709,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>41938</v>
       </c>
@@ -2751,7 +2753,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>41938</v>
       </c>
@@ -2795,7 +2797,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>41938</v>
       </c>
@@ -2839,7 +2841,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2880,7 +2882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>41940</v>
       </c>
@@ -2921,7 +2923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>41940</v>
       </c>
@@ -2962,7 +2964,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>41940</v>
       </c>
@@ -3006,7 +3008,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>41941</v>
       </c>
@@ -3050,7 +3052,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>41941</v>
       </c>
@@ -3094,7 +3096,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>41941</v>
       </c>
@@ -3138,7 +3140,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>41942</v>
       </c>
@@ -3179,7 +3181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>41942</v>
       </c>
@@ -3223,7 +3225,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>41942</v>
       </c>
@@ -3264,7 +3266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>41942</v>
       </c>
@@ -3308,7 +3310,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>41942</v>
       </c>
@@ -3352,7 +3354,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>41942</v>
       </c>
@@ -3396,7 +3398,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>41943</v>
       </c>
@@ -3440,7 +3442,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>41943</v>
       </c>
@@ -3484,7 +3486,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>41943</v>
       </c>
@@ -3528,7 +3530,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>41943</v>
       </c>
@@ -3572,7 +3574,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>41943</v>
       </c>
@@ -3616,7 +3618,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>41945</v>
       </c>
@@ -3660,7 +3662,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>41945</v>
       </c>
@@ -3701,7 +3703,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>41948</v>
       </c>
@@ -3745,7 +3747,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>41948</v>
       </c>
@@ -3786,7 +3788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>41949</v>
       </c>
@@ -3827,7 +3829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>41949</v>
       </c>
@@ -3868,7 +3870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>41949</v>
       </c>
@@ -3912,7 +3914,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>41949</v>
       </c>
@@ -3956,7 +3958,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>41950</v>
       </c>
@@ -4000,7 +4002,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>41950</v>
       </c>
@@ -4044,7 +4046,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>41950</v>
       </c>
@@ -4088,7 +4090,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>41950</v>
       </c>
@@ -4132,7 +4134,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>41950</v>
       </c>
@@ -4176,7 +4178,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>41950</v>
       </c>
@@ -4217,10 +4219,10 @@
         <v>15</v>
       </c>
       <c r="N81" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>41952</v>
       </c>
@@ -4228,7 +4230,7 @@
         <v>0.5</v>
       </c>
       <c r="C82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D82">
         <v>137</v>
@@ -4264,7 +4266,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>41952</v>
       </c>
@@ -4305,10 +4307,10 @@
         <v>10</v>
       </c>
       <c r="N83" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>41952</v>
       </c>
@@ -4349,10 +4351,10 @@
         <v>18</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>41954</v>
       </c>
@@ -4393,10 +4395,10 @@
         <v>10</v>
       </c>
       <c r="N85" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>41954</v>
       </c>
@@ -4437,10 +4439,10 @@
         <v>15</v>
       </c>
       <c r="N86" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>41954</v>
       </c>
@@ -4481,7 +4483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>41954</v>
       </c>
@@ -4522,7 +4524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>41955</v>
       </c>
@@ -4530,7 +4532,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C89" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D89">
         <v>143</v>
@@ -4563,10 +4565,10 @@
         <v>15</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>41955</v>
       </c>
@@ -4607,10 +4609,10 @@
         <v>10</v>
       </c>
       <c r="N90" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>41955</v>
       </c>
@@ -4651,7 +4653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>41956</v>
       </c>
@@ -4692,7 +4694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>41956</v>
       </c>
@@ -4733,7 +4735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>41956</v>
       </c>
@@ -4774,10 +4776,10 @@
         <v>15</v>
       </c>
       <c r="N94" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>41956</v>
       </c>
@@ -4785,7 +4787,7 @@
         <v>0.71875</v>
       </c>
       <c r="C95" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D95">
         <v>149</v>
@@ -4818,10 +4820,10 @@
         <v>10</v>
       </c>
       <c r="N95" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>41956</v>
       </c>
@@ -4862,10 +4864,10 @@
         <v>10</v>
       </c>
       <c r="N96" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>41959</v>
       </c>
@@ -4873,7 +4875,7 @@
         <v>0.5</v>
       </c>
       <c r="C97" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -4883,24 +4885,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Writing, editing, code tidying.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Note_sheet_AM.xlsx
+++ b/raw-data-prep/raw_data/Note_sheet_AM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -302,34 +302,34 @@
     <t>Study about effect of distraction on video game playing. Anything suspicious: maybe we were writing the essay responses to distract the more. laughed when gave distraction assignment. Said essay review was too much. A normal person isn't that mean.</t>
   </si>
   <si>
-    <t>Game 2</t>
-  </si>
-  <si>
-    <t>Game 4</t>
-  </si>
-  <si>
-    <t>Game 6</t>
-  </si>
-  <si>
-    <t>Good Session</t>
-  </si>
-  <si>
     <t>Notes_t</t>
   </si>
   <si>
-    <t>Game 1</t>
-  </si>
-  <si>
-    <t>Game 3</t>
-  </si>
-  <si>
-    <t>Game 5</t>
+    <t>Game.1</t>
+  </si>
+  <si>
+    <t>Game.2</t>
+  </si>
+  <si>
+    <t>Game.3</t>
+  </si>
+  <si>
+    <t>Game.4</t>
+  </si>
+  <si>
+    <t>Game.5</t>
+  </si>
+  <si>
+    <t>Game.6</t>
+  </si>
+  <si>
+    <t>goodSession</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -500,7 +500,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,7 +535,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -748,7 +748,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8:M8"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,28 +777,28 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" t="s">
         <v>91</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" t="s">
         <v>86</v>
-      </c>
-      <c r="I1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" t="s">
-        <v>89</v>
-      </c>
-      <c r="N1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed date-time info. -added a package dependency.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Note_sheet_AM.xlsx
+++ b/raw-data-prep/raw_data/Note_sheet_AM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="170" windowWidth="14810" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="91">
   <si>
     <t>Subject</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Participant a little weird; Stood up to ask about how to move on in game; was opening up drawers when I came into room; Results would've been different, no challenge to game- kind of boring</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Seems okay</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
   </si>
   <si>
     <t>Not sure how much of essay prompt was understood; did seem to understand the process of judging essays was fake- learned about similar studies previously; English as a second language - I allowed him to use phone to translate</t>
-  </si>
-  <si>
-    <t>9/?</t>
   </si>
   <si>
     <t>JH</t>
@@ -197,9 +191,6 @@
     <t>Thought it was about exactly what we said it was about</t>
   </si>
   <si>
-    <t xml:space="preserve"> 10/28</t>
-  </si>
-  <si>
     <t>Thought we were interested in seing how he responded to his partner's feedback but he believed he was paired with the other participant</t>
   </si>
   <si>
@@ -329,7 +320,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,21 +416,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -500,7 +492,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,7 +527,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -747,17 +739,18 @@
   <dimension ref="A1:N97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:M1"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -777,35 +770,35 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" t="s">
         <v>87</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>88</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>89</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>90</v>
       </c>
-      <c r="K1" t="s">
-        <v>91</v>
-      </c>
-      <c r="L1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M1" t="s">
-        <v>93</v>
-      </c>
       <c r="N1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5">
         <v>41541</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="11">
         <v>0.70833333333333337</v>
       </c>
       <c r="C2" t="s">
@@ -838,18 +831,18 @@
       <c r="L2">
         <v>0</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    <row r="3" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
         <v>41541</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="11">
         <v>0.70833333333333337</v>
       </c>
       <c r="C3" t="s">
@@ -886,11 +879,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
         <v>41541</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="11">
         <v>0.75</v>
       </c>
       <c r="C4" t="s">
@@ -927,11 +920,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
         <v>41542</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="11">
         <v>0.71875</v>
       </c>
       <c r="C5" t="s">
@@ -964,18 +957,18 @@
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
         <v>41542</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="11">
         <v>0.71875</v>
       </c>
       <c r="C6" t="s">
@@ -1012,15 +1005,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
         <v>41543</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="11">
         <v>0.64583333333333337</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -1053,11 +1046,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
         <v>41543</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="11">
         <v>0.64583333333333337</v>
       </c>
       <c r="C8" t="s">
@@ -1090,15 +1083,13 @@
       <c r="L8">
         <v>60</v>
       </c>
-      <c r="M8" s="11"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
         <v>41543</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
+      <c r="B9" s="11"/>
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -1129,20 +1120,20 @@
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9" s="11"/>
+      <c r="M9" s="8"/>
       <c r="N9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
         <v>41543</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="11">
         <v>0.6875</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -1175,11 +1166,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="5">
         <v>41543</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="11">
         <v>0.72916666666666663</v>
       </c>
       <c r="C11" t="s">
@@ -1216,15 +1207,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+    <row r="12" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="5">
         <v>41543</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="11">
         <v>0.72916666666666663</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12">
         <v>12</v>
@@ -1253,15 +1244,15 @@
       <c r="L12">
         <v>91</v>
       </c>
-      <c r="M12" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="M12" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
         <v>41544</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="11">
         <v>0.58333333333333337</v>
       </c>
       <c r="C13" t="s">
@@ -1298,18 +1289,18 @@
         <v>14</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="5">
         <v>41544</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="11">
         <v>0.58333333333333337</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14">
         <v>14</v>
@@ -1342,14 +1333,14 @@
         <v>14</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="5">
         <v>41545</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="11">
         <v>0.50208333333333333</v>
       </c>
       <c r="C15" t="s">
@@ -1382,22 +1373,22 @@
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15" s="13" t="s">
+      <c r="M15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+    <row r="16" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5">
         <v>41545</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="11">
         <v>0.5</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16">
         <v>16</v>
@@ -1430,18 +1421,16 @@
         <v>14</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="5"/>
+      <c r="B17" s="11">
         <v>0.58333333333333337</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D17">
         <v>18</v>
@@ -1470,18 +1459,18 @@
       <c r="L17">
         <v>73</v>
       </c>
-      <c r="M17" s="8" t="s">
+      <c r="M17" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="5">
         <v>41545</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="11">
         <v>0.58333333333333337</v>
       </c>
       <c r="C18" t="s">
@@ -1521,15 +1510,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="5">
         <v>41545</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="11">
         <v>0.58333333333333337</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19">
         <v>20</v>
@@ -1558,22 +1547,22 @@
       <c r="L19">
         <v>65</v>
       </c>
-      <c r="M19" s="8" t="s">
+      <c r="M19" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="5">
+        <v>41546</v>
+      </c>
+      <c r="B20" s="11">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C20" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>41546</v>
-      </c>
-      <c r="B20" s="10">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C20" t="s">
-        <v>32</v>
       </c>
       <c r="D20">
         <v>21</v>
@@ -1602,22 +1591,22 @@
       <c r="L20">
         <v>0</v>
       </c>
-      <c r="M20" s="8" t="s">
+      <c r="M20" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="5">
         <v>41546</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="11">
         <v>0.54166666666666663</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D21">
         <v>22</v>
@@ -1650,14 +1639,14 @@
         <v>9</v>
       </c>
       <c r="N21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="5">
         <v>41547</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="11">
         <v>0.71875</v>
       </c>
       <c r="C22" t="s">
@@ -1694,14 +1683,14 @@
         <v>9</v>
       </c>
       <c r="N22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="5">
         <v>41547</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="11">
         <v>0.71875</v>
       </c>
       <c r="C23" t="s">
@@ -1738,11 +1727,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="5">
         <v>41548</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="11">
         <v>0.75</v>
       </c>
       <c r="C24" t="s">
@@ -1779,11 +1768,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="5">
         <v>41548</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="11">
         <v>0.70833333333333337</v>
       </c>
       <c r="C25" t="s">
@@ -1816,22 +1805,18 @@
       <c r="L25">
         <v>55</v>
       </c>
-      <c r="M25" s="8" t="s">
+      <c r="M25" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" t="s">
-        <v>20</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" s="5"/>
+      <c r="B26" s="11"/>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D26">
         <v>27</v>
@@ -1864,11 +1849,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="5">
         <v>41548</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="11">
         <v>0.63541666666666663</v>
       </c>
       <c r="C27" t="s">
@@ -1901,18 +1886,18 @@
       <c r="L27">
         <v>74</v>
       </c>
-      <c r="M27" s="8" t="s">
+      <c r="M27" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="5">
         <v>41549</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="11">
         <v>0.67708333333333337</v>
       </c>
       <c r="C28" t="s">
@@ -1949,13 +1934,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>20</v>
-      </c>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" s="5"/>
+      <c r="B29" s="11"/>
       <c r="C29" t="s">
         <v>8</v>
       </c>
@@ -1990,11 +1971,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" s="5">
         <v>41549</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="11">
         <v>0.67708333333333337</v>
       </c>
       <c r="C30" t="s">
@@ -2031,11 +2012,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" s="5">
         <v>41549</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="11">
         <v>0.71875</v>
       </c>
       <c r="C31" t="s">
@@ -2072,14 +2053,14 @@
         <v>9</v>
       </c>
       <c r="N31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" s="5">
         <v>41550</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="11">
         <v>0.64583333333333337</v>
       </c>
       <c r="C32" t="s">
@@ -2112,17 +2093,17 @@
       <c r="L32">
         <v>0</v>
       </c>
-      <c r="M32" s="11"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+      <c r="M32" s="8"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A33" s="5">
         <v>41550</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="11">
         <v>0.64583333333333337</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D33">
         <v>34</v>
@@ -2155,15 +2136,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
+    <row r="34" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="5">
         <v>41550</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="11">
         <v>0.6875</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D34">
         <v>36</v>
@@ -2196,11 +2177,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3">
+    <row r="35" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="5">
         <v>41550</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="11">
         <v>0.72916666666666663</v>
       </c>
       <c r="C35" t="s">
@@ -2233,20 +2214,20 @@
       <c r="L35">
         <v>0</v>
       </c>
-      <c r="M35" s="12"/>
-      <c r="N35" s="5" t="s">
+      <c r="M35" s="9"/>
+      <c r="N35" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+    <row r="36" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5">
         <v>41550</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="11">
         <v>0.72916666666666663</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D36">
         <v>38</v>
@@ -2279,11 +2260,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A37" s="5">
         <v>41550</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="11">
         <v>0.77083333333333337</v>
       </c>
       <c r="C37" t="s">
@@ -2320,15 +2301,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A38" s="5">
         <v>41550</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="11">
         <v>0.77083333333333337</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D38">
         <v>40</v>
@@ -2361,14 +2342,14 @@
         <v>9</v>
       </c>
       <c r="N38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A39" s="5">
         <v>41551</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="11">
         <v>0.58333333333333337</v>
       </c>
       <c r="C39" t="s">
@@ -2405,15 +2386,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3">
+    <row r="40" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="5">
         <v>41551</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="11">
         <v>0.58333333333333337</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D40">
         <v>42</v>
@@ -2446,14 +2427,14 @@
         <v>9</v>
       </c>
       <c r="N40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="5">
         <v>41551</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="11">
         <v>0.625</v>
       </c>
       <c r="C41" t="s">
@@ -2488,15 +2469,15 @@
       </c>
       <c r="M41" s="2"/>
     </row>
-    <row r="42" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
+    <row r="42" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="5">
         <v>41936</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="11">
         <v>0.6875</v>
       </c>
       <c r="C42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D42">
         <v>95</v>
@@ -2529,18 +2510,16 @@
         <v>9</v>
       </c>
       <c r="N42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A43" s="5">
         <v>41936</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="B43" s="11"/>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D43">
         <v>96</v>
@@ -2573,18 +2552,18 @@
         <v>14</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A44" s="5">
         <v>41936</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="11">
         <v>0.72916666666666663</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D44">
         <v>97</v>
@@ -2617,18 +2596,18 @@
         <v>9</v>
       </c>
       <c r="N44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A45" s="5">
         <v>41936</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="11">
         <v>0.73611111111111116</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D45">
         <v>98</v>
@@ -2661,18 +2640,18 @@
         <v>9</v>
       </c>
       <c r="N45" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A46" s="5">
         <v>41936</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="11">
         <v>0.77083333333333337</v>
       </c>
       <c r="C46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D46">
         <v>99</v>
@@ -2705,14 +2684,14 @@
         <v>9</v>
       </c>
       <c r="N46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A47" s="5">
         <v>41938</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="11">
         <v>0.54583333333333328</v>
       </c>
       <c r="C47" t="s">
@@ -2745,22 +2724,22 @@
       <c r="L47">
         <v>23</v>
       </c>
-      <c r="M47" s="8" t="s">
+      <c r="M47" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A48" s="5">
+        <v>41938</v>
+      </c>
+      <c r="B48" s="11">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C48" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <v>41938</v>
-      </c>
-      <c r="B48" s="6">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="C48" t="s">
-        <v>49</v>
       </c>
       <c r="D48">
         <v>101</v>
@@ -2793,16 +2772,14 @@
         <v>9</v>
       </c>
       <c r="N48" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A49" s="5">
         <v>41938</v>
       </c>
-      <c r="B49" t="s">
-        <v>20</v>
-      </c>
+      <c r="B49" s="11"/>
       <c r="C49" t="s">
         <v>13</v>
       </c>
@@ -2837,14 +2814,14 @@
         <v>9</v>
       </c>
       <c r="N49" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A50" s="5">
         <v>41940</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50" s="11">
         <v>0.70833333333333337</v>
       </c>
       <c r="C50" t="s">
@@ -2881,11 +2858,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="6">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A51" s="5">
+        <v>41940</v>
+      </c>
+      <c r="B51" s="11">
         <v>0.70833333333333337</v>
       </c>
       <c r="C51" t="s">
@@ -2922,11 +2899,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A52" s="5">
         <v>41940</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="11">
         <v>0.75</v>
       </c>
       <c r="C52" t="s">
@@ -2963,11 +2940,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A53" s="5">
         <v>41940</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" s="11">
         <v>0.75</v>
       </c>
       <c r="C53" t="s">
@@ -3004,14 +2981,14 @@
         <v>9</v>
       </c>
       <c r="N53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A54" s="5">
         <v>41941</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="11">
         <v>0.70833333333333337</v>
       </c>
       <c r="C54" t="s">
@@ -3048,14 +3025,14 @@
         <v>9</v>
       </c>
       <c r="N54" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A55" s="5">
         <v>41941</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="11">
         <v>0.70833333333333337</v>
       </c>
       <c r="C55" t="s">
@@ -3092,14 +3069,14 @@
         <v>14</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A56" s="5">
         <v>41941</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="11">
         <v>0.75</v>
       </c>
       <c r="C56" t="s">
@@ -3136,14 +3113,14 @@
         <v>9</v>
       </c>
       <c r="N56" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A57" s="5">
         <v>41942</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="11">
         <v>0.63541666666666663</v>
       </c>
       <c r="C57" t="s">
@@ -3180,15 +3157,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A58" s="5">
         <v>41942</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58" s="11">
         <v>0.63541666666666663</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D58">
         <v>111</v>
@@ -3217,18 +3194,18 @@
       <c r="L58">
         <v>0</v>
       </c>
-      <c r="M58" s="8" t="s">
+      <c r="M58" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N58" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A59" s="5">
         <v>41942</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="11">
         <v>0.67708333333333337</v>
       </c>
       <c r="C59" t="s">
@@ -3265,15 +3242,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A60" s="5">
         <v>41942</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="11">
         <v>0.67708333333333337</v>
       </c>
       <c r="C60" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D60">
         <v>113</v>
@@ -3306,14 +3283,14 @@
         <v>9</v>
       </c>
       <c r="N60" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A61" s="5">
         <v>41942</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61" s="11">
         <v>0.71875</v>
       </c>
       <c r="C61" t="s">
@@ -3350,18 +3327,18 @@
         <v>9</v>
       </c>
       <c r="N61" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A62" s="5">
         <v>41942</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62" s="11">
         <v>0.71875</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D62">
         <v>115</v>
@@ -3394,18 +3371,18 @@
         <v>9</v>
       </c>
       <c r="N62" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A63" s="5">
         <v>41943</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" s="11">
         <v>0.64583333333333337</v>
       </c>
       <c r="C63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D63">
         <v>116</v>
@@ -3438,18 +3415,18 @@
         <v>9</v>
       </c>
       <c r="N63" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A64" s="5">
         <v>41943</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64" s="11">
         <v>0.72916666666666663</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D64">
         <v>118</v>
@@ -3478,22 +3455,22 @@
       <c r="L64">
         <v>68</v>
       </c>
-      <c r="M64" s="8" t="s">
-        <v>62</v>
+      <c r="M64" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="N64" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A65" s="5">
         <v>41943</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65" s="11">
         <v>0.72916666666666663</v>
       </c>
       <c r="C65" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D65">
         <v>119</v>
@@ -3526,18 +3503,18 @@
         <v>14</v>
       </c>
       <c r="N65" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A66" s="5">
         <v>41943</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="11">
         <v>0.77083333333333337</v>
       </c>
       <c r="C66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D66">
         <v>120</v>
@@ -3570,20 +3547,20 @@
         <v>9</v>
       </c>
       <c r="N66" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A67" s="5">
         <v>41943</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67" s="11">
         <v>0.77083333333333337</v>
       </c>
       <c r="C67" t="s">
-        <v>42</v>
-      </c>
-      <c r="D67" s="9">
+        <v>40</v>
+      </c>
+      <c r="D67" s="7">
         <v>121</v>
       </c>
       <c r="E67">
@@ -3614,14 +3591,14 @@
         <v>9</v>
       </c>
       <c r="N67" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A68" s="5">
         <v>41945</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68" s="11">
         <v>0.5</v>
       </c>
       <c r="C68" t="s">
@@ -3658,18 +3635,18 @@
         <v>9</v>
       </c>
       <c r="N68" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A69" s="5">
         <v>41945</v>
       </c>
-      <c r="B69" s="6">
+      <c r="B69" s="11">
         <v>0.5</v>
       </c>
       <c r="C69" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D69">
         <v>123</v>
@@ -3702,11 +3679,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A70" s="5">
         <v>41948</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70" s="11">
         <v>0.70833333333333337</v>
       </c>
       <c r="C70" t="s">
@@ -3743,14 +3720,14 @@
         <v>9</v>
       </c>
       <c r="N70" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A71" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A71" s="5">
         <v>41948</v>
       </c>
-      <c r="B71" s="6">
+      <c r="B71" s="11">
         <v>0.75</v>
       </c>
       <c r="C71" t="s">
@@ -3787,11 +3764,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A72" s="3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A72" s="5">
         <v>41949</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" s="11">
         <v>0.63541666666666663</v>
       </c>
       <c r="C72" t="s">
@@ -3828,11 +3805,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A73" s="3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A73" s="5">
         <v>41949</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B73" s="11">
         <v>0.63541666666666663</v>
       </c>
       <c r="C73" t="s">
@@ -3869,11 +3846,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" s="3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A74" s="5">
         <v>41949</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="11">
         <v>0.67708333333333337</v>
       </c>
       <c r="C74" t="s">
@@ -3910,14 +3887,14 @@
         <v>9</v>
       </c>
       <c r="N74" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A75" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A75" s="5">
         <v>41949</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B75" s="11">
         <v>0.71875</v>
       </c>
       <c r="C75" t="s">
@@ -3954,18 +3931,18 @@
         <v>14</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A76" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A76" s="5">
         <v>41950</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="11">
         <v>0.64583333333333337</v>
       </c>
       <c r="C76" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D76">
         <v>130</v>
@@ -3998,18 +3975,18 @@
         <v>9</v>
       </c>
       <c r="N76" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A77" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A77" s="5">
         <v>41950</v>
       </c>
-      <c r="B77" s="6">
+      <c r="B77" s="11">
         <v>0.64583333333333337</v>
       </c>
       <c r="C77" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D77">
         <v>131</v>
@@ -4038,22 +4015,22 @@
       <c r="L77">
         <v>0</v>
       </c>
-      <c r="M77" s="8" t="s">
+      <c r="M77" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N77" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A78" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A78" s="5">
         <v>41950</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78" s="11">
         <v>0.6875</v>
       </c>
       <c r="C78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D78">
         <v>132</v>
@@ -4086,18 +4063,18 @@
         <v>9</v>
       </c>
       <c r="N78" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A79" s="3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A79" s="5">
         <v>41950</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B79" s="11">
         <v>0.6875</v>
       </c>
       <c r="C79" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D79">
         <v>133</v>
@@ -4126,22 +4103,22 @@
       <c r="L79">
         <v>0</v>
       </c>
-      <c r="M79" s="8" t="s">
+      <c r="M79" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N79" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A80" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A80" s="5">
         <v>41950</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B80" s="11">
         <v>0.72916666666666663</v>
       </c>
       <c r="C80" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D80">
         <v>134</v>
@@ -4170,22 +4147,22 @@
       <c r="L80">
         <v>74</v>
       </c>
-      <c r="M80" s="8" t="s">
+      <c r="M80" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N80" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A81" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A81" s="5">
         <v>41950</v>
       </c>
-      <c r="B81" s="6">
+      <c r="B81" s="11">
         <v>0.72916666666666663</v>
       </c>
       <c r="C81" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D81">
         <v>135</v>
@@ -4218,18 +4195,18 @@
         <v>9</v>
       </c>
       <c r="N81" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A82" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A82" s="5">
         <v>41952</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="11">
         <v>0.5</v>
       </c>
       <c r="C82" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D82">
         <v>136</v>
@@ -4262,18 +4239,18 @@
         <v>9</v>
       </c>
       <c r="N82" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A83" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A83" s="5">
         <v>41952</v>
       </c>
-      <c r="B83" s="6">
+      <c r="B83" s="11">
         <v>0.5</v>
       </c>
       <c r="C83" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D83">
         <v>137</v>
@@ -4306,18 +4283,16 @@
         <v>9</v>
       </c>
       <c r="N83" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A84" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A84" s="5">
         <v>41952</v>
       </c>
-      <c r="B84" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="B84" s="11"/>
       <c r="C84" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D84">
         <v>138</v>
@@ -4350,14 +4325,14 @@
         <v>14</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" s="3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A85" s="5">
         <v>41954</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B85" s="11">
         <v>0.70833333333333337</v>
       </c>
       <c r="C85" t="s">
@@ -4394,14 +4369,14 @@
         <v>9</v>
       </c>
       <c r="N85" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A86" s="3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A86" s="5">
         <v>41954</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="11">
         <v>0.70833333333333337</v>
       </c>
       <c r="C86" t="s">
@@ -4434,18 +4409,18 @@
       <c r="L86">
         <v>150</v>
       </c>
-      <c r="M86" s="8" t="s">
+      <c r="M86" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N86" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A87" s="5">
         <v>41954</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87" s="11">
         <v>0.75</v>
       </c>
       <c r="C87" t="s">
@@ -4482,11 +4457,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A88" s="3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A88" s="5">
         <v>41954</v>
       </c>
-      <c r="B88" s="6">
+      <c r="B88" s="11">
         <v>0.75</v>
       </c>
       <c r="C88" t="s">
@@ -4523,15 +4498,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A89" s="3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A89" s="5">
         <v>41955</v>
       </c>
-      <c r="B89" s="6">
+      <c r="B89" s="11">
         <v>0.70833333333333337</v>
       </c>
       <c r="C89" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D89">
         <v>143</v>
@@ -4560,18 +4535,18 @@
       <c r="L89">
         <v>0</v>
       </c>
-      <c r="M89" s="8" t="s">
+      <c r="M89" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A90" s="3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A90" s="5">
         <v>41955</v>
       </c>
-      <c r="B90" s="6">
+      <c r="B90" s="11">
         <v>0.70833333333333337</v>
       </c>
       <c r="C90" t="s">
@@ -4608,14 +4583,14 @@
         <v>9</v>
       </c>
       <c r="N90" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A91" s="3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A91" s="5">
         <v>41955</v>
       </c>
-      <c r="B91" s="6">
+      <c r="B91" s="11">
         <v>0.75</v>
       </c>
       <c r="C91" t="s">
@@ -4652,11 +4627,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A92" s="3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A92" s="5">
         <v>41956</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92" s="11">
         <v>0.63541666666666663</v>
       </c>
       <c r="C92" t="s">
@@ -4693,11 +4668,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A93" s="3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A93" s="5">
         <v>41956</v>
       </c>
-      <c r="B93" s="6">
+      <c r="B93" s="11">
         <v>0.63541666666666663</v>
       </c>
       <c r="C93" t="s">
@@ -4734,11 +4709,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A94" s="3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A94" s="5">
         <v>41956</v>
       </c>
-      <c r="B94" s="6">
+      <c r="B94" s="11">
         <v>0.67708333333333337</v>
       </c>
       <c r="C94" t="s">
@@ -4771,22 +4746,22 @@
       <c r="L94">
         <v>65</v>
       </c>
-      <c r="M94" s="8" t="s">
+      <c r="M94" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N94" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A95" s="3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A95" s="5">
         <v>41956</v>
       </c>
-      <c r="B95" s="6">
+      <c r="B95" s="11">
         <v>0.71875</v>
       </c>
       <c r="C95" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D95">
         <v>149</v>
@@ -4819,14 +4794,14 @@
         <v>9</v>
       </c>
       <c r="N95" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A96" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A96" s="5">
         <v>41956</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B96" s="11">
         <v>0.71875</v>
       </c>
       <c r="C96" t="s">
@@ -4863,18 +4838,18 @@
         <v>9</v>
       </c>
       <c r="N96" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="5">
         <v>41959</v>
       </c>
-      <c r="B97" s="10">
+      <c r="B97" s="11">
         <v>0.5</v>
       </c>
       <c r="C97" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -4894,7 +4869,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4906,7 +4881,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>